<commit_message>
Added delay and disaster recovery
</commit_message>
<xml_diff>
--- a/Portfolio of Applications Business Model 5yr.xlsx
+++ b/Portfolio of Applications Business Model 5yr.xlsx
@@ -5,31 +5,32 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsubda/git/containerization-and-cloud-economic-model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsubda/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246A0672-FFEF-F648-9989-D09590184895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A59216C8-DE2B-3C41-8401-49B0E6073287}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="860" windowWidth="25900" windowHeight="14960" firstSheet="10" activeTab="14" xr2:uid="{9EB35D73-6E70-F94A-8F74-E60F0DF94BAF}"/>
+    <workbookView xWindow="0" yWindow="840" windowWidth="25900" windowHeight="14960" xr2:uid="{9EB35D73-6E70-F94A-8F74-E60F0DF94BAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="5" r:id="rId1"/>
     <sheet name="Yearly Savings" sheetId="18" r:id="rId2"/>
     <sheet name="Yearly Values &amp; Costs" sheetId="12" r:id="rId3"/>
     <sheet name="Portfolio Value Summary" sheetId="11" r:id="rId4"/>
-    <sheet name="Portfolio Cost Summary" sheetId="7" r:id="rId5"/>
-    <sheet name="Team Hourly Burn" sheetId="10" r:id="rId6"/>
-    <sheet name="Sensitivity Analysis Variables" sheetId="9" r:id="rId7"/>
-    <sheet name="Sensitity Analysis Constants" sheetId="6" r:id="rId8"/>
-    <sheet name="Sensitity Analysis Dropdowns" sheetId="8" r:id="rId9"/>
-    <sheet name="ValCnst(Legacy-&gt;Containerized)" sheetId="13" r:id="rId10"/>
-    <sheet name="CostCnst(Legacy-&gt;Containerized)" sheetId="1" r:id="rId11"/>
-    <sheet name="CostOpts(Legacy-&gt;Containerized)" sheetId="3" r:id="rId12"/>
-    <sheet name="CostCnst(Containerized-&gt;Cloud)" sheetId="2" r:id="rId13"/>
-    <sheet name="Cost Constants" sheetId="4" r:id="rId14"/>
-    <sheet name="Value Constants" sheetId="14" r:id="rId15"/>
+    <sheet name="Value Constants" sheetId="14" r:id="rId5"/>
+    <sheet name="Portfolio Cost Summary" sheetId="7" r:id="rId6"/>
+    <sheet name="Team Hourly Burn" sheetId="10" r:id="rId7"/>
+    <sheet name="Sensitivity Analysis Variables" sheetId="9" r:id="rId8"/>
+    <sheet name="Sensitity Analysis Constants" sheetId="6" r:id="rId9"/>
+    <sheet name="Sensitity Analysis Dropdowns" sheetId="8" r:id="rId10"/>
+    <sheet name="ValCnst(Legacy-&gt;Containerized)" sheetId="13" r:id="rId11"/>
+    <sheet name="CostCnst(Legacy-&gt;Containerized)" sheetId="1" r:id="rId12"/>
+    <sheet name="CostOpts(Legacy-&gt;Containerized)" sheetId="3" r:id="rId13"/>
+    <sheet name="CostCnst(Containerized-&gt;Cloud)" sheetId="2" r:id="rId14"/>
+    <sheet name="Cost Constants" sheetId="4" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="183">
   <si>
     <t>Data Changes</t>
   </si>
@@ -476,6 +477,126 @@
   </si>
   <si>
     <t>2017 data, global security survey, Subscription Research</t>
+  </si>
+  <si>
+    <t>Division of effort per experience on OpenShift platform teams</t>
+  </si>
+  <si>
+    <t>https://www.effective-software.com/blog/5-financial-benefits-of-moving-to-the-cloud</t>
+  </si>
+  <si>
+    <t>Average Disaster Recovery Time for Businesses Running on Non-Cloud Infrastructure</t>
+  </si>
+  <si>
+    <t>Average Disaster Recovery Time for Businesses Running on Cloud Infrastructure</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>Likelihood of a Design Event Earthquake in BC</t>
+  </si>
+  <si>
+    <t>https://www.egbc.ca/getmedia/4278c069-0374-4cc2-9e73-2b454a0f978a/SEABC-Eathquake-Fact-Sheet.pdf.aspx</t>
+  </si>
+  <si>
+    <t>Likelihood of one of Disaster Recover level datacenter events</t>
+  </si>
+  <si>
+    <t>chance/year</t>
+  </si>
+  <si>
+    <t>ransomware, fire, virus, network, storm, workforce stoppages, terrorist attacks, vandalism, flooding, cyberattack - https://invenioit.com/continuity/4-real-life-business-continuity-examples/</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/221592515_Comparative_Analysis_of_Job_Satisfaction_in_Agile_and_Non-agile_Software_Development_Teams</t>
+  </si>
+  <si>
+    <t>Retention Multiplier Due to Switch from Waterfall to Agile</t>
+  </si>
+  <si>
+    <t>Tech Sector Turnover Rate</t>
+  </si>
+  <si>
+    <t>https://www.informationweek.com/strategic-cio/team-building-and-staffing/whats-driving-the-tech-sectors-extreme-turnover-rate/a/d-id/1334920</t>
+  </si>
+  <si>
+    <t>Average Time to Fill a Role in IT Recruiting</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>Time to Create a New Posting</t>
+  </si>
+  <si>
+    <t>Staff Involved in Creating Posting</t>
+  </si>
+  <si>
+    <t>staff</t>
+  </si>
+  <si>
+    <t>1 Senior Technology Staff Member, 1 Ministry HR Staff Member, 1 Public Service Staff Member (PSA)</t>
+  </si>
+  <si>
+    <t>Time to Review Applicants (Initial Submissions) by PSA/HR</t>
+  </si>
+  <si>
+    <t>Assume average 50 submissions</t>
+  </si>
+  <si>
+    <t>Time to Review Filtered Applicants</t>
+  </si>
+  <si>
+    <t>Assume 20 applications pass initial screening</t>
+  </si>
+  <si>
+    <t>Creation of Candidate Test</t>
+  </si>
+  <si>
+    <t>Assume taking previous tests and modifying them so as not to reuse exact questions/tasks</t>
+  </si>
+  <si>
+    <t>Code Challenge over the course of a week including weekend</t>
+  </si>
+  <si>
+    <t>Application of Candidate Test including Review</t>
+  </si>
+  <si>
+    <t>Candidate in Person Interviews</t>
+  </si>
+  <si>
+    <t>Assume 3 to 5 finalists</t>
+  </si>
+  <si>
+    <t>Number of Staff on Interview Panel</t>
+  </si>
+  <si>
+    <t>Post Selection Activities (Records Management, Feedback Calls, Announcements)</t>
+  </si>
+  <si>
+    <t>Onboarding New Staff Member</t>
+  </si>
+  <si>
+    <t>Introductions, equipment, forms, keycards, facilities tour.  Other specific training left to the Project Team</t>
+  </si>
+  <si>
+    <t>Average Cost of Turnover as a Percentage of Employee Salary</t>
+  </si>
+  <si>
+    <t>https://blogs.oracle.com/smb/4-sure-fire-ways-oracle-hcm-cloud-boosts-productivity</t>
+  </si>
+  <si>
+    <t>Improved Technologist Retention factor due to working on modern technologies</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Delay Factor due to half-year conversion time</t>
+  </si>
+  <si>
+    <t>Assume it takes 6 months for the conversion work to be done and for any values &amp; savings to take effect</t>
   </si>
 </sst>
 </file>
@@ -557,7 +678,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -582,19 +703,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -736,19 +858,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>250052.21551842181</c:v>
+                  <c:v>125376.5729438198</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>472409.08500184363</c:v>
+                  <c:v>376129.71883145947</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>917122.82396868733</c:v>
+                  <c:v>877636.01060673862</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1806550.3019023745</c:v>
+                  <c:v>1880648.5941572969</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3585405.257769749</c:v>
+                  <c:v>3886673.761258414</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1314,19 +1436,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>106276.44246872517</c:v>
+                  <c:v>-18399.200105876836</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>184857.53890245035</c:v>
+                  <c:v>88578.172732066188</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>342019.73176990077</c:v>
+                  <c:v>302532.91840795206</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>656344.11750480137</c:v>
+                  <c:v>730442.40975972381</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1284992.8889746028</c:v>
+                  <c:v>1586261.3924632678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3027,11 +3149,11 @@
   </sheetPr>
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3186,9 +3308,12 @@
       </c>
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E26" t="s">
+      <c r="E26" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
     </row>
     <row r="44" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I44" s="3"/>
@@ -3260,6 +3385,252 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D477174F-5EB3-D14B-80D0-DCACDF5B81EF}">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B5" sqref="B5:F5"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5:F5"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:F5"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="55.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731DAEB7-84E3-F64E-A6D2-57429C6FFEA3}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -3289,7 +3660,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21880609-280D-7840-884C-B6D9F6A39CDD}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3363,7 +3734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCAD7EB-2781-E14C-90C6-B0A74EB91CBA}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3406,7 +3777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4DB2EF4-5C6D-0F4E-9382-000FC8FE0D80}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3480,7 +3851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C2EF97-D034-D047-982A-FFFC278580D2}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3491,7 +3862,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3618,343 +3989,6 @@
       </c>
       <c r="D9" t="s">
         <v>98</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505FF6CF-6A1B-6E42-BA01-A0AFAB15D317}">
-  <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:D27"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="72.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="11">
-        <v>31.828099999999999</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="4">
-        <f>2.3/7.9</f>
-        <v>0.29113924050632906</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1.40923</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1460000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="5">
-        <f>B5/B4</f>
-        <v>1036026.7663901564</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="5">
-        <v>4440000</v>
-      </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="5">
-        <f>B7*B3*B4</f>
-        <v>1821652.7544303793</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="7">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="D9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="7">
-        <v>0.16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="7">
-        <f>B9*B10</f>
-        <v>9.2799999999999994E-2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="7">
-        <f>177/430</f>
-        <v>0.41162790697674417</v>
-      </c>
-      <c r="D12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0.98</v>
-      </c>
-      <c r="D15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="D16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>136</v>
-      </c>
-      <c r="B17" s="12">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>138</v>
-      </c>
-      <c r="D17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B18" s="12">
-        <f>30</f>
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" s="6">
-        <v>0.72</v>
-      </c>
-      <c r="D19" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>111</v>
-      </c>
-      <c r="B20" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>112</v>
-      </c>
-      <c r="B21" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B22" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="12">
-        <v>3</v>
-      </c>
-      <c r="D23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" s="12">
-        <v>24</v>
-      </c>
-      <c r="D24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="6">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>127</v>
-      </c>
-      <c r="B26" s="6">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="6">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -3992,7 +4026,7 @@
       </c>
       <c r="B2" s="19">
         <f>'Yearly Values &amp; Costs'!B2-'Yearly Values &amp; Costs'!C2</f>
-        <v>106276.44246872517</v>
+        <v>-18399.200105876836</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4001,7 +4035,7 @@
       </c>
       <c r="B3" s="19">
         <f>'Yearly Values &amp; Costs'!B3-'Yearly Values &amp; Costs'!C3</f>
-        <v>184857.53890245035</v>
+        <v>88578.172732066188</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -4010,7 +4044,7 @@
       </c>
       <c r="B4" s="19">
         <f>'Yearly Values &amp; Costs'!B4-'Yearly Values &amp; Costs'!C4</f>
-        <v>342019.73176990077</v>
+        <v>302532.91840795206</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -4019,7 +4053,7 @@
       </c>
       <c r="B5" s="19">
         <f>'Yearly Values &amp; Costs'!B5-'Yearly Values &amp; Costs'!C5</f>
-        <v>656344.11750480137</v>
+        <v>730442.40975972381</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -4028,7 +4062,7 @@
       </c>
       <c r="B6" s="19">
         <f>'Yearly Values &amp; Costs'!B6-'Yearly Values &amp; Costs'!C6</f>
-        <v>1284992.8889746028</v>
+        <v>1586261.3924632678</v>
       </c>
     </row>
   </sheetData>
@@ -4077,8 +4111,8 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <f>'Portfolio Value Summary'!$C$22</f>
-        <v>250052.21551842181</v>
+        <f>'Portfolio Value Summary'!$C$23</f>
+        <v>125376.5729438198</v>
       </c>
       <c r="C2" s="1">
         <f>'Portfolio Cost Summary'!$C$13</f>
@@ -4086,7 +4120,7 @@
       </c>
       <c r="D2" s="17">
         <f>B2-C2</f>
-        <v>106276.44246872517</v>
+        <v>-18399.200105876836</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4094,16 +4128,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <f>'Portfolio Value Summary'!$D$22</f>
-        <v>472409.08500184363</v>
+        <f>'Portfolio Value Summary'!$D$23</f>
+        <v>376129.71883145947</v>
       </c>
       <c r="C3" s="1">
         <f>'Portfolio Cost Summary'!$D$13</f>
         <v>287551.54609939328</v>
       </c>
       <c r="D3" s="17">
-        <f t="shared" ref="D3:D6" si="0">B3-C3</f>
-        <v>184857.53890245035</v>
+        <f>B3-C3</f>
+        <v>88578.172732066188</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4111,16 +4145,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <f>'Portfolio Value Summary'!$E$22</f>
-        <v>917122.82396868733</v>
+        <f>'Portfolio Value Summary'!$E$23</f>
+        <v>877636.01060673862</v>
       </c>
       <c r="C4" s="1">
         <f>'Portfolio Cost Summary'!$E$13</f>
         <v>575103.09219878656</v>
       </c>
       <c r="D4" s="17">
-        <f t="shared" si="0"/>
-        <v>342019.73176990077</v>
+        <f>B4-C4</f>
+        <v>302532.91840795206</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4128,16 +4162,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <f>'Portfolio Value Summary'!$F$22</f>
-        <v>1806550.3019023745</v>
+        <f>'Portfolio Value Summary'!$F$23</f>
+        <v>1880648.5941572969</v>
       </c>
       <c r="C5" s="1">
         <f>'Portfolio Cost Summary'!$F$13</f>
         <v>1150206.1843975731</v>
       </c>
       <c r="D5" s="17">
-        <f t="shared" si="0"/>
-        <v>656344.11750480137</v>
+        <f>B5-C5</f>
+        <v>730442.40975972381</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4145,16 +4179,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <f>'Portfolio Value Summary'!$G$22</f>
-        <v>3585405.257769749</v>
+        <f>'Portfolio Value Summary'!$G$23</f>
+        <v>3886673.761258414</v>
       </c>
       <c r="C6" s="1">
         <f>'Portfolio Cost Summary'!$G$13</f>
         <v>2300412.3687951462</v>
       </c>
       <c r="D6" s="17">
-        <f t="shared" si="0"/>
-        <v>1284992.8889746028</v>
+        <f>B6-C6</f>
+        <v>1586261.3924632678</v>
       </c>
     </row>
     <row r="27" spans="5:5" x14ac:dyDescent="0.2">
@@ -4170,14 +4204,14 @@
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M28" sqref="M28"/>
       <selection pane="topRight" activeCell="M28" sqref="M28"/>
       <selection pane="bottomLeft" activeCell="M28" sqref="M28"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4244,7 +4278,7 @@
         <v>802278.9281216244</v>
       </c>
       <c r="H2" s="11">
-        <f>SUM(C2:G2)</f>
+        <f t="shared" ref="H2:H22" si="0">SUM(C2:G2)</f>
         <v>1554415.4232356474</v>
       </c>
     </row>
@@ -4276,7 +4310,7 @@
         <v>56795.367365599988</v>
       </c>
       <c r="H3" s="11">
-        <f t="shared" ref="H3" si="0">SUM(C3:G3)</f>
+        <f t="shared" si="0"/>
         <v>110041.02427084997</v>
       </c>
     </row>
@@ -4308,7 +4342,7 @@
         <v>4431255.3656000001</v>
       </c>
       <c r="H4" s="11">
-        <f>SUM(C4:G4)</f>
+        <f t="shared" si="0"/>
         <v>8585557.270849999</v>
       </c>
     </row>
@@ -4340,7 +4374,7 @@
         <v>2215627.6828000001</v>
       </c>
       <c r="H5" s="11">
-        <f t="shared" ref="H5:H7" si="1">SUM(C5:G5)</f>
+        <f t="shared" si="0"/>
         <v>4292778.6354249995</v>
       </c>
     </row>
@@ -4372,7 +4406,7 @@
         <v>1329376.60968</v>
       </c>
       <c r="H6" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2575667.1812549997</v>
       </c>
     </row>
@@ -4404,40 +4438,40 @@
         <v>886251.07312000007</v>
       </c>
       <c r="H7" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1717111.4541700003</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C8" s="11">
-        <f>C2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>22564.094853420684</v>
+        <f>(('Value Constants'!$B$17*'Team Hourly Burn'!$B$2)+('Value Constants'!$B$18*'Cost Constants'!$B$4)+('Sensitivity Analysis Variables'!$C$8*'Sensitivity Analysis Variables'!$C$10))*'Value Constants'!$B$28*'Sensitivity Analysis Variables'!C$3*(SUM('Value Constants'!$B$30,'Value Constants'!$B$31))</f>
+        <v>950.41405995633659</v>
       </c>
       <c r="D8" s="11">
-        <f>D2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>45128.189706841367</v>
+        <f>(('Value Constants'!$B$17*'Team Hourly Burn'!$B$2)+('Value Constants'!$B$18*'Cost Constants'!$B$4)+('Sensitivity Analysis Variables'!$C$8*'Sensitivity Analysis Variables'!$C$10))*'Value Constants'!$B$28*'Sensitivity Analysis Variables'!D$3*(SUM('Value Constants'!$B$30,'Value Constants'!$B$31))</f>
+        <v>1900.8281199126732</v>
       </c>
       <c r="E8" s="11">
-        <f>E2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>90256.379413682735</v>
+        <f>(('Value Constants'!$B$17*'Team Hourly Burn'!$B$2)+('Value Constants'!$B$18*'Cost Constants'!$B$4)+('Sensitivity Analysis Variables'!$C$8*'Sensitivity Analysis Variables'!$C$10))*'Value Constants'!$B$28*'Sensitivity Analysis Variables'!E$3*(SUM('Value Constants'!$B$30,'Value Constants'!$B$31))</f>
+        <v>3801.6562398253463</v>
       </c>
       <c r="F8" s="11">
-        <f>F2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>180512.75882736547</v>
+        <f>(('Value Constants'!$B$17*'Team Hourly Burn'!$B$2)+('Value Constants'!$B$18*'Cost Constants'!$B$4)+('Sensitivity Analysis Variables'!$C$8*'Sensitivity Analysis Variables'!$C$10))*'Value Constants'!$B$28*'Sensitivity Analysis Variables'!F$3*(SUM('Value Constants'!$B$30,'Value Constants'!$B$31))</f>
+        <v>7603.3124796506927</v>
       </c>
       <c r="G8" s="11">
-        <f>G2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>361025.51765473094</v>
+        <f>(('Value Constants'!$B$17*'Team Hourly Burn'!$B$2)+('Value Constants'!$B$18*'Cost Constants'!$B$4)+('Sensitivity Analysis Variables'!$C$8*'Sensitivity Analysis Variables'!$C$10))*'Value Constants'!$B$28*'Sensitivity Analysis Variables'!G$3*(SUM('Value Constants'!$B$30,'Value Constants'!$B$31))</f>
+        <v>15206.624959301385</v>
       </c>
       <c r="H8" s="11">
-        <f>SUM(C8:G8)</f>
-        <v>699486.94045604113</v>
+        <f t="shared" si="0"/>
+        <v>29462.835858646435</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -4445,31 +4479,31 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="C9" s="11">
-        <f>C$5*'Value Constants'!$B$20</f>
-        <v>110781.38414000001</v>
+        <f>(C$2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47</f>
+        <v>11282.047426710342</v>
       </c>
       <c r="D9" s="11">
-        <f>D$5*'Value Constants'!$B$20</f>
-        <v>221562.76828000002</v>
+        <f>C$9+((D$2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>33846.142280131025</v>
       </c>
       <c r="E9" s="11">
-        <f>E$5*'Value Constants'!$B$20</f>
-        <v>443125.53656000004</v>
+        <f>D$9+((E$2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>78974.331986972393</v>
       </c>
       <c r="F9" s="11">
-        <f>F$5*'Value Constants'!$B$20</f>
-        <v>886251.07312000007</v>
+        <f>E$9+((F$2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>169230.71140065513</v>
       </c>
       <c r="G9" s="11">
-        <f>G$5*'Value Constants'!$B$20</f>
-        <v>1772502.1462400001</v>
+        <f>F$9+((G$2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>349743.47022802057</v>
       </c>
       <c r="H9" s="11">
-        <f t="shared" ref="H9:H20" si="2">SUM(C9:G9)</f>
-        <v>3434222.9083400005</v>
+        <f t="shared" si="0"/>
+        <v>643076.70332248951</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -4477,31 +4511,31 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" s="11">
-        <f>C$6*'Value Constants'!$B$21</f>
-        <v>49851.622862999997</v>
+        <f>(C$5*'Value Constants'!$B$20)/'Value Constants'!$B$47</f>
+        <v>55390.692070000005</v>
       </c>
       <c r="D10" s="11">
-        <f>D$6*'Value Constants'!$B$21</f>
-        <v>99703.245725999994</v>
+        <f>C$10+((D$5*'Value Constants'!$B$20)/'Value Constants'!$B$47)</f>
+        <v>166172.07621000003</v>
       </c>
       <c r="E10" s="11">
-        <f>E$6*'Value Constants'!$B$21</f>
-        <v>199406.49145199999</v>
+        <f>D$10+((E$5*'Value Constants'!$B$20)/'Value Constants'!$B$47)</f>
+        <v>387734.84449000005</v>
       </c>
       <c r="F10" s="11">
-        <f>F$6*'Value Constants'!$B$21</f>
-        <v>398812.98290399997</v>
+        <f>E$10+((F$5*'Value Constants'!$B$20)/'Value Constants'!$B$47)</f>
+        <v>830860.38105000008</v>
       </c>
       <c r="G10" s="11">
-        <f>G$6*'Value Constants'!$B$21</f>
-        <v>797625.96580799995</v>
+        <f>F$10+((G$5*'Value Constants'!$B$20)/'Value Constants'!$B$47)</f>
+        <v>1717111.4541700003</v>
       </c>
       <c r="H10" s="11">
-        <f>SUM(C10:G10)</f>
-        <v>1545400.3087529999</v>
+        <f t="shared" si="0"/>
+        <v>3157269.4479900002</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -4509,31 +4543,31 @@
         <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C11" s="11">
-        <f>$C$7*'Value Constants'!$B$22</f>
-        <v>27695.346035000002</v>
+        <f>(C$6*'Value Constants'!$B$21)/'Value Constants'!$B$47</f>
+        <v>24925.811431499998</v>
       </c>
       <c r="D11" s="11">
-        <f>$C$7*'Value Constants'!$B$22</f>
-        <v>27695.346035000002</v>
+        <f>C$11+((D$6*'Value Constants'!$B$21)/'Value Constants'!$B$47)</f>
+        <v>74777.434294499995</v>
       </c>
       <c r="E11" s="11">
-        <f>$C$7*'Value Constants'!$B$22</f>
-        <v>27695.346035000002</v>
+        <f>D$11+((E$6*'Value Constants'!$B$21)/'Value Constants'!$B$47)</f>
+        <v>174480.68002049997</v>
       </c>
       <c r="F11" s="11">
-        <f>$C$7*'Value Constants'!$B$22</f>
-        <v>27695.346035000002</v>
+        <f>E$11+((F$6*'Value Constants'!$B$21)/'Value Constants'!$B$47)</f>
+        <v>373887.17147249996</v>
       </c>
       <c r="G11" s="11">
-        <f>$C$7*'Value Constants'!$B$22</f>
-        <v>27695.346035000002</v>
+        <f>F$11+((G$6*'Value Constants'!$B$21)/'Value Constants'!$B$47)</f>
+        <v>772700.15437649994</v>
       </c>
       <c r="H11" s="11">
-        <f t="shared" si="2"/>
-        <v>138476.730175</v>
+        <f t="shared" si="0"/>
+        <v>1420771.2515954999</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -4541,87 +4575,99 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+        <v>101</v>
+      </c>
+      <c r="C12" s="11">
+        <f>(C$7*'Value Constants'!$B$22)/'Value Constants'!$B$47</f>
+        <v>13847.673017500001</v>
+      </c>
+      <c r="D12" s="11">
+        <f>C$12+((D$7*'Value Constants'!$B$22)/'Value Constants'!$B$47)</f>
+        <v>41543.019052500007</v>
+      </c>
+      <c r="E12" s="11">
+        <f>D$12+((E$7*'Value Constants'!$B$22)/'Value Constants'!$B$47)</f>
+        <v>96933.711122500012</v>
+      </c>
+      <c r="F12" s="11">
+        <f>E$12+((F$7*'Value Constants'!$B$22)/'Value Constants'!$B$47)</f>
+        <v>207715.09526250002</v>
+      </c>
+      <c r="G12" s="11">
+        <f>F$12+((G$7*'Value Constants'!$B$22)/'Value Constants'!$B$47)</f>
+        <v>429277.86354250007</v>
+      </c>
+      <c r="H12" s="11">
+        <f t="shared" si="0"/>
+        <v>789317.36199750006</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="H13" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="H14" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+      <c r="H15" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="11">
-        <f>C2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>36603.976095549115</v>
-      </c>
-      <c r="D16" s="11">
-        <f>D2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>73207.952191098229</v>
-      </c>
-      <c r="E16" s="11">
-        <f>E2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>146415.90438219646</v>
-      </c>
-      <c r="F16" s="11">
-        <f>F2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>292831.80876439292</v>
-      </c>
-      <c r="G16" s="11">
-        <f>G2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>585663.61752878584</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="11">
-        <f t="shared" si="2"/>
-        <v>1134723.2589620226</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -4629,31 +4675,31 @@
         <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="C17" s="11">
-        <f>'Portfolio Value Summary'!C$3*'Value Constants'!$B$19</f>
-        <v>2555.7915314519992</v>
+        <f>(C$2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47</f>
+        <v>18301.988047774557</v>
       </c>
       <c r="D17" s="11">
-        <f>'Portfolio Value Summary'!D$3*'Value Constants'!$B$19</f>
-        <v>5111.5830629039983</v>
+        <f>C$17+((D$2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>54905.964143323668</v>
       </c>
       <c r="E17" s="11">
-        <f>'Portfolio Value Summary'!E$3*'Value Constants'!$B$19</f>
-        <v>10223.166125807997</v>
+        <f>D$17+((E$2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>128113.9163344219</v>
       </c>
       <c r="F17" s="11">
-        <f>'Portfolio Value Summary'!F$3*'Value Constants'!$B$19</f>
-        <v>20446.332251615993</v>
+        <f>E$17+((F$2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>274529.82071661833</v>
       </c>
       <c r="G17" s="11">
-        <f>'Portfolio Value Summary'!G$3*'Value Constants'!$B$19</f>
-        <v>40892.664503231987</v>
+        <f>F$17+((G$2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>567361.6294810113</v>
       </c>
       <c r="H17" s="11">
-        <f>SUM(C17:G17)</f>
-        <v>79229.537475011981</v>
+        <f t="shared" si="0"/>
+        <v>1043213.3187231498</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -4661,16 +4707,31 @@
         <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+        <v>129</v>
+      </c>
+      <c r="C18" s="11">
+        <f>('Portfolio Value Summary'!C$3*'Value Constants'!$B$19)/'Value Constants'!$B$47</f>
+        <v>1277.8957657259996</v>
+      </c>
+      <c r="D18" s="11">
+        <f>C$18+(('Portfolio Value Summary'!D$3*'Value Constants'!$B$19)/'Value Constants'!$B$47)</f>
+        <v>3833.6872971779985</v>
+      </c>
+      <c r="E18" s="11">
+        <f>D$18+(('Portfolio Value Summary'!E$3*'Value Constants'!$B$19)/'Value Constants'!$B$47)</f>
+        <v>8945.2703600819968</v>
+      </c>
+      <c r="F18" s="11">
+        <f>E$18+(('Portfolio Value Summary'!F$3*'Value Constants'!$B$19)/'Value Constants'!$B$47)</f>
+        <v>19168.436485889993</v>
+      </c>
+      <c r="G18" s="11">
+        <f>F$18+(('Portfolio Value Summary'!G$3*'Value Constants'!$B$19)/'Value Constants'!$B$47)</f>
+        <v>39614.76873750599</v>
+      </c>
       <c r="H18" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>72840.058646381978</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -4678,16 +4739,31 @@
         <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+        <v>102</v>
+      </c>
+      <c r="C19" s="11">
+        <f>((1-('Value Constants'!$B$29/'Value Constants'!$B$28))*'Portfolio Value Summary'!C$8)/'Value Constants'!$B$47</f>
+        <v>350.46518460889916</v>
+      </c>
+      <c r="D19" s="11">
+        <f>C$19+(((1-('Value Constants'!$B$29/'Value Constants'!$B$28))*'Portfolio Value Summary'!D$8)/'Value Constants'!$B$47)</f>
+        <v>1051.3955538266976</v>
+      </c>
+      <c r="E19" s="11">
+        <f>D$19+(((1-('Value Constants'!$B$29/'Value Constants'!$B$28))*'Portfolio Value Summary'!E$8)/'Value Constants'!$B$47)</f>
+        <v>2453.2562922622942</v>
+      </c>
+      <c r="F19" s="11">
+        <f>E$19+(((1-('Value Constants'!$B$29/'Value Constants'!$B$28))*'Portfolio Value Summary'!F$8)/'Value Constants'!$B$47)</f>
+        <v>5256.9777691334875</v>
+      </c>
+      <c r="G19" s="11">
+        <f>F$19+(((1-('Value Constants'!$B$29/'Value Constants'!$B$28))*'Portfolio Value Summary'!G$8)/'Value Constants'!$B$47)</f>
+        <v>10864.420722875875</v>
+      </c>
       <c r="H19" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>19976.515522707254</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -4695,7 +4771,7 @@
         <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -4703,7 +4779,7 @@
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -4712,42 +4788,62 @@
         <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
+      <c r="H21" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="11">
-        <f>SUM(C8:C20)</f>
-        <v>250052.21551842181</v>
-      </c>
-      <c r="D22" s="11">
-        <f>SUM(D8:D20)</f>
-        <v>472409.08500184363</v>
-      </c>
-      <c r="E22" s="11">
-        <f>SUM(E8:E20)</f>
-        <v>917122.82396868733</v>
-      </c>
-      <c r="F22" s="11">
-        <f>SUM(F8:F20)</f>
-        <v>1806550.3019023745</v>
-      </c>
-      <c r="G22" s="11">
-        <f>SUM(G8:G20)</f>
-        <v>3585405.257769749</v>
-      </c>
-      <c r="H22" s="11">
-        <f>SUM(C22:G22)</f>
-        <v>7031539.6841610763</v>
+      <c r="C23" s="11">
+        <f>SUM(C9:C21)</f>
+        <v>125376.5729438198</v>
+      </c>
+      <c r="D23" s="11">
+        <f>SUM(D9:D21)</f>
+        <v>376129.71883145947</v>
+      </c>
+      <c r="E23" s="11">
+        <f>SUM(E9:E21)</f>
+        <v>877636.01060673862</v>
+      </c>
+      <c r="F23" s="11">
+        <f>SUM(F9:F21)</f>
+        <v>1880648.5941572969</v>
+      </c>
+      <c r="G23" s="11">
+        <f>SUM(G9:G21)</f>
+        <v>3886673.761258414</v>
+      </c>
+      <c r="H23" s="11">
+        <f>SUM(C23:G23)</f>
+        <v>7146464.6577977287</v>
       </c>
     </row>
   </sheetData>
@@ -4756,6 +4852,607 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505FF6CF-6A1B-6E42-BA01-A0AFAB15D317}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:D47"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B47" sqref="B47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="72.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="11">
+        <v>31.828099999999999</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="4">
+        <f>2.3/7.9</f>
+        <v>0.29113924050632906</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1.40923</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1460000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="5">
+        <f>B5/B4</f>
+        <v>1036026.7663901564</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="5">
+        <v>4440000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="5">
+        <f>B7*B3*B4</f>
+        <v>1821652.7544303793</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="7">
+        <f>B9*B10</f>
+        <v>9.2799999999999994E-2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="7">
+        <f>177/430</f>
+        <v>0.41162790697674417</v>
+      </c>
+      <c r="D12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0.98</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="D16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="12">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" s="12">
+        <f>30</f>
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="D19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="12">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="12">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>145</v>
+      </c>
+      <c r="B28" s="12">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>147</v>
+      </c>
+      <c r="D28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="12">
+        <v>2.1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30">
+        <f>1/2475</f>
+        <v>4.0404040404040404E-4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>151</v>
+      </c>
+      <c r="D30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="12">
+        <f>1/10</f>
+        <v>0.1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B32" s="12">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="20">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="D33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="12">
+        <v>51</v>
+      </c>
+      <c r="C34" t="s">
+        <v>158</v>
+      </c>
+      <c r="D34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35" s="12">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>160</v>
+      </c>
+      <c r="B36" s="12">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="12">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>165</v>
+      </c>
+      <c r="B38" s="12">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="12">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>170</v>
+      </c>
+      <c r="B40" s="12">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>171</v>
+      </c>
+      <c r="B41" s="12">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>173</v>
+      </c>
+      <c r="B42" s="12">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B43" s="12">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" s="12">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>181</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D4432B-F9B7-BD4A-9D67-F31606253D99}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -5177,19 +5874,19 @@
         <v>143775.77304969664</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="D13:G13" si="1">SUM(D2:D12)</f>
+        <f>SUM(D2:D12)</f>
         <v>287551.54609939328</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="1"/>
+        <f>SUM(E2:E12)</f>
         <v>575103.09219878656</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
+        <f>SUM(F2:F12)</f>
         <v>1150206.1843975731</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="1"/>
+        <f>SUM(G2:G12)</f>
         <v>2300412.3687951462</v>
       </c>
       <c r="H13" s="1">
@@ -5202,7 +5899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1226F3-B512-544C-9A73-84F0129838E2}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -5244,7 +5941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6621B249-8CC2-E94D-9485-1BC74B88D830}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -5268,13 +5965,13 @@
       <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -5338,14 +6035,14 @@
         <f>Dashboard!$C3</f>
         <v>10% Employees</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="21">
         <f>IF('Sensitity Analysis Dropdowns'!$B$5='Sensitivity Analysis Variables'!$B4, 'Sensitity Analysis Constants'!$B$5, IF('Sensitity Analysis Dropdowns'!$B$6='Sensitivity Analysis Variables'!$B4, 'Sensitity Analysis Constants'!$B$6, 'Sensitity Analysis Constants'!$B$7))</f>
         <v>0.1</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
@@ -5356,14 +6053,14 @@
         <f>Dashboard!$C4</f>
         <v>Trained by Working on Previous Teams</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="21">
         <f>IF('Sensitity Analysis Dropdowns'!$B$8='Sensitivity Analysis Variables'!$B5, 'Sensitity Analysis Constants'!$B$8, IF('Sensitity Analysis Dropdowns'!$B$9='Sensitivity Analysis Variables'!$B5, 'Sensitity Analysis Constants'!$B$9, 'Sensitity Analysis Constants'!$B$10))</f>
         <v>1</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
@@ -5374,14 +6071,14 @@
         <f>Dashboard!$C5</f>
         <v>Medium</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="21">
         <f>IF('Sensitity Analysis Dropdowns'!$B$11='Sensitivity Analysis Variables'!$B6, 'Sensitity Analysis Constants'!$B$11, IF('Sensitity Analysis Dropdowns'!$B$12='Sensitivity Analysis Variables'!$B6, 'Sensitity Analysis Constants'!$B$12, 'Sensitity Analysis Constants'!$B$13))</f>
         <v>0.65</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
@@ -5410,14 +6107,14 @@
         <f>Dashboard!$C7</f>
         <v>5</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="23">
         <f>IF('Sensitity Analysis Dropdowns'!$B$17='Sensitivity Analysis Variables'!$B8, 'Sensitity Analysis Constants'!B$17, IF('Sensitity Analysis Dropdowns'!$B$18='Sensitivity Analysis Variables'!$B8, 'Sensitity Analysis Constants'!$B$18, 'Sensitity Analysis Constants'!$B$19))</f>
         <v>5</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
@@ -5428,14 +6125,14 @@
         <f>Dashboard!$C8</f>
         <v>3 hours</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="23">
         <f>IF('Sensitity Analysis Dropdowns'!$B$20='Sensitivity Analysis Variables'!$B9, 'Sensitity Analysis Constants'!B$20, IF('Sensitity Analysis Dropdowns'!$B$21='Sensitivity Analysis Variables'!$B9, 'Sensitity Analysis Constants'!B21, 'Sensitity Analysis Constants'!B22))</f>
         <v>3</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
@@ -5464,14 +6161,14 @@
         <f>Dashboard!$C10</f>
         <v>Low (3000)</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="21">
         <f>IF('Sensitity Analysis Dropdowns'!$B$26='Sensitivity Analysis Variables'!$B11, 'Sensitity Analysis Constants'!B$26, IF('Sensitity Analysis Dropdowns'!$B$27='Sensitivity Analysis Variables'!$B11, 'Sensitity Analysis Constants'!$B$27, 'Sensitity Analysis Constants'!$B$28))</f>
         <v>3000</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5489,7 +6186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1E70E2-DD7C-2F49-82BE-73E99E27C39B}">
   <dimension ref="A1:H28"/>
   <sheetViews>
@@ -5539,15 +6236,15 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:F2" si="0">C2*2</f>
+        <f>C2*2</f>
         <v>4</v>
       </c>
       <c r="E2">
-        <f t="shared" si="0"/>
+        <f>D2*2</f>
         <v>8</v>
       </c>
       <c r="F2">
-        <f t="shared" si="0"/>
+        <f>E2*2</f>
         <v>16</v>
       </c>
       <c r="H2" t="s">
@@ -5563,19 +6260,19 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:F4" si="1">B3*2</f>
+        <f t="shared" ref="C3:F4" si="0">B3*2</f>
         <v>4</v>
       </c>
       <c r="D3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="H3" t="s">
@@ -5591,19 +6288,19 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
@@ -5615,10 +6312,10 @@
       <c r="B5" s="24">
         <v>0.1</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
@@ -5628,10 +6325,10 @@
       <c r="B6" s="24">
         <v>0.5</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
@@ -5641,49 +6338,49 @@
       <c r="B7" s="24">
         <v>0.9</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A8, " - ", 'Sensitity Analysis Dropdowns'!$B8)</f>
         <v>Experience of Teams with BC Gov Migrations - Figuring it out from Scratch</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="21">
         <v>1.5</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A9, " - ", 'Sensitity Analysis Dropdowns'!$B9)</f>
         <v>Experience of Teams with BC Gov Migrations - Following Best Practice Documents</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="21">
         <v>1.3</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A10, " - ", 'Sensitity Analysis Dropdowns'!$B10)</f>
         <v>Experience of Teams with BC Gov Migrations - Trained by Working on Previous Teams</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="21">
         <v>1</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
@@ -5693,10 +6390,10 @@
       <c r="B11" s="24">
         <v>0.25</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
@@ -5706,10 +6403,10 @@
       <c r="B12" s="24">
         <v>0.65</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
@@ -5719,10 +6416,10 @@
       <c r="B13" s="24">
         <v>0.9</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
@@ -5743,14 +6440,14 @@
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A15, " - ", 'Sensitity Analysis Dropdowns'!$B15)</f>
         <v>Average Cost of Gov Data Breach - Medium</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="25">
         <f>($B$16+$B$14)/2</f>
         <v>1640826.3772151896</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
@@ -5771,78 +6468,78 @@
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A17, " - ", 'Sensitity Analysis Dropdowns'!$B17)</f>
         <v>Average Currently Online Public Users per Application - 5</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="23">
         <v>5</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A18, " - ", 'Sensitity Analysis Dropdowns'!$B18)</f>
         <v>Average Currently Online Public Users per Application - 20</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="23">
         <v>20</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A19, " - ", 'Sensitity Analysis Dropdowns'!$B19)</f>
         <v>Average Currently Online Public Users per Application - 100</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="23">
         <v>100</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A20, " - ", 'Sensitity Analysis Dropdowns'!$B20)</f>
         <v>Average Legacy System Outage Length - 3 hours</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="23">
         <v>3</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A21, " - ", 'Sensitity Analysis Dropdowns'!$B21)</f>
         <v>Average Legacy System Outage Length - 10 hours</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="23">
         <v>10</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A22, " - ", 'Sensitity Analysis Dropdowns'!$B22)</f>
         <v>Average Legacy System Outage Length - 100 hours</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="23">
         <v>100</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
@@ -5888,313 +6585,67 @@
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A26, " - ", 'Sensitity Analysis Dropdowns'!$B26)</f>
         <v>Average Yearly Project Hours on New Features - Low (3000)</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="21">
         <v>3000</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A27, " - ", 'Sensitity Analysis Dropdowns'!$B27)</f>
         <v>Average Yearly Project Hours on New Features - Medium (7500)</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="21">
         <v>7500</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A28, " - ", 'Sensitity Analysis Dropdowns'!$B28)</f>
         <v>Average Yearly Project Hours on New Features - High (12000)</v>
       </c>
-      <c r="B28" s="20">
+      <c r="B28" s="21">
         <v>12000</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D477174F-5EB3-D14B-80D0-DCACDF5B81EF}">
-  <dimension ref="A1:B28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B5" sqref="B5:F5"/>
-      <selection pane="topRight" activeCell="B5" sqref="B5:F5"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5:F5"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="55.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>135</v>
-      </c>
-      <c r="B19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>131</v>
-      </c>
-      <c r="B20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>131</v>
-      </c>
-      <c r="B21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>131</v>
-      </c>
-      <c r="B22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" s="15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>130</v>
-      </c>
-      <c r="B24" s="15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" s="15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>121</v>
-      </c>
-      <c r="B26" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>121</v>
-      </c>
-      <c r="B27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added delay and disaster recovery (#8)
</commit_message>
<xml_diff>
--- a/Portfolio of Applications Business Model 5yr.xlsx
+++ b/Portfolio of Applications Business Model 5yr.xlsx
@@ -5,31 +5,32 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsubda/git/containerization-and-cloud-economic-model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsubda/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246A0672-FFEF-F648-9989-D09590184895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A59216C8-DE2B-3C41-8401-49B0E6073287}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="860" windowWidth="25900" windowHeight="14960" firstSheet="10" activeTab="14" xr2:uid="{9EB35D73-6E70-F94A-8F74-E60F0DF94BAF}"/>
+    <workbookView xWindow="0" yWindow="840" windowWidth="25900" windowHeight="14960" xr2:uid="{9EB35D73-6E70-F94A-8F74-E60F0DF94BAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="5" r:id="rId1"/>
     <sheet name="Yearly Savings" sheetId="18" r:id="rId2"/>
     <sheet name="Yearly Values &amp; Costs" sheetId="12" r:id="rId3"/>
     <sheet name="Portfolio Value Summary" sheetId="11" r:id="rId4"/>
-    <sheet name="Portfolio Cost Summary" sheetId="7" r:id="rId5"/>
-    <sheet name="Team Hourly Burn" sheetId="10" r:id="rId6"/>
-    <sheet name="Sensitivity Analysis Variables" sheetId="9" r:id="rId7"/>
-    <sheet name="Sensitity Analysis Constants" sheetId="6" r:id="rId8"/>
-    <sheet name="Sensitity Analysis Dropdowns" sheetId="8" r:id="rId9"/>
-    <sheet name="ValCnst(Legacy-&gt;Containerized)" sheetId="13" r:id="rId10"/>
-    <sheet name="CostCnst(Legacy-&gt;Containerized)" sheetId="1" r:id="rId11"/>
-    <sheet name="CostOpts(Legacy-&gt;Containerized)" sheetId="3" r:id="rId12"/>
-    <sheet name="CostCnst(Containerized-&gt;Cloud)" sheetId="2" r:id="rId13"/>
-    <sheet name="Cost Constants" sheetId="4" r:id="rId14"/>
-    <sheet name="Value Constants" sheetId="14" r:id="rId15"/>
+    <sheet name="Value Constants" sheetId="14" r:id="rId5"/>
+    <sheet name="Portfolio Cost Summary" sheetId="7" r:id="rId6"/>
+    <sheet name="Team Hourly Burn" sheetId="10" r:id="rId7"/>
+    <sheet name="Sensitivity Analysis Variables" sheetId="9" r:id="rId8"/>
+    <sheet name="Sensitity Analysis Constants" sheetId="6" r:id="rId9"/>
+    <sheet name="Sensitity Analysis Dropdowns" sheetId="8" r:id="rId10"/>
+    <sheet name="ValCnst(Legacy-&gt;Containerized)" sheetId="13" r:id="rId11"/>
+    <sheet name="CostCnst(Legacy-&gt;Containerized)" sheetId="1" r:id="rId12"/>
+    <sheet name="CostOpts(Legacy-&gt;Containerized)" sheetId="3" r:id="rId13"/>
+    <sheet name="CostCnst(Containerized-&gt;Cloud)" sheetId="2" r:id="rId14"/>
+    <sheet name="Cost Constants" sheetId="4" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="183">
   <si>
     <t>Data Changes</t>
   </si>
@@ -476,6 +477,126 @@
   </si>
   <si>
     <t>2017 data, global security survey, Subscription Research</t>
+  </si>
+  <si>
+    <t>Division of effort per experience on OpenShift platform teams</t>
+  </si>
+  <si>
+    <t>https://www.effective-software.com/blog/5-financial-benefits-of-moving-to-the-cloud</t>
+  </si>
+  <si>
+    <t>Average Disaster Recovery Time for Businesses Running on Non-Cloud Infrastructure</t>
+  </si>
+  <si>
+    <t>Average Disaster Recovery Time for Businesses Running on Cloud Infrastructure</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>Likelihood of a Design Event Earthquake in BC</t>
+  </si>
+  <si>
+    <t>https://www.egbc.ca/getmedia/4278c069-0374-4cc2-9e73-2b454a0f978a/SEABC-Eathquake-Fact-Sheet.pdf.aspx</t>
+  </si>
+  <si>
+    <t>Likelihood of one of Disaster Recover level datacenter events</t>
+  </si>
+  <si>
+    <t>chance/year</t>
+  </si>
+  <si>
+    <t>ransomware, fire, virus, network, storm, workforce stoppages, terrorist attacks, vandalism, flooding, cyberattack - https://invenioit.com/continuity/4-real-life-business-continuity-examples/</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/221592515_Comparative_Analysis_of_Job_Satisfaction_in_Agile_and_Non-agile_Software_Development_Teams</t>
+  </si>
+  <si>
+    <t>Retention Multiplier Due to Switch from Waterfall to Agile</t>
+  </si>
+  <si>
+    <t>Tech Sector Turnover Rate</t>
+  </si>
+  <si>
+    <t>https://www.informationweek.com/strategic-cio/team-building-and-staffing/whats-driving-the-tech-sectors-extreme-turnover-rate/a/d-id/1334920</t>
+  </si>
+  <si>
+    <t>Average Time to Fill a Role in IT Recruiting</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>Time to Create a New Posting</t>
+  </si>
+  <si>
+    <t>Staff Involved in Creating Posting</t>
+  </si>
+  <si>
+    <t>staff</t>
+  </si>
+  <si>
+    <t>1 Senior Technology Staff Member, 1 Ministry HR Staff Member, 1 Public Service Staff Member (PSA)</t>
+  </si>
+  <si>
+    <t>Time to Review Applicants (Initial Submissions) by PSA/HR</t>
+  </si>
+  <si>
+    <t>Assume average 50 submissions</t>
+  </si>
+  <si>
+    <t>Time to Review Filtered Applicants</t>
+  </si>
+  <si>
+    <t>Assume 20 applications pass initial screening</t>
+  </si>
+  <si>
+    <t>Creation of Candidate Test</t>
+  </si>
+  <si>
+    <t>Assume taking previous tests and modifying them so as not to reuse exact questions/tasks</t>
+  </si>
+  <si>
+    <t>Code Challenge over the course of a week including weekend</t>
+  </si>
+  <si>
+    <t>Application of Candidate Test including Review</t>
+  </si>
+  <si>
+    <t>Candidate in Person Interviews</t>
+  </si>
+  <si>
+    <t>Assume 3 to 5 finalists</t>
+  </si>
+  <si>
+    <t>Number of Staff on Interview Panel</t>
+  </si>
+  <si>
+    <t>Post Selection Activities (Records Management, Feedback Calls, Announcements)</t>
+  </si>
+  <si>
+    <t>Onboarding New Staff Member</t>
+  </si>
+  <si>
+    <t>Introductions, equipment, forms, keycards, facilities tour.  Other specific training left to the Project Team</t>
+  </si>
+  <si>
+    <t>Average Cost of Turnover as a Percentage of Employee Salary</t>
+  </si>
+  <si>
+    <t>https://blogs.oracle.com/smb/4-sure-fire-ways-oracle-hcm-cloud-boosts-productivity</t>
+  </si>
+  <si>
+    <t>Improved Technologist Retention factor due to working on modern technologies</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Delay Factor due to half-year conversion time</t>
+  </si>
+  <si>
+    <t>Assume it takes 6 months for the conversion work to be done and for any values &amp; savings to take effect</t>
   </si>
 </sst>
 </file>
@@ -557,7 +678,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -582,19 +703,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -736,19 +858,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>250052.21551842181</c:v>
+                  <c:v>125376.5729438198</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>472409.08500184363</c:v>
+                  <c:v>376129.71883145947</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>917122.82396868733</c:v>
+                  <c:v>877636.01060673862</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1806550.3019023745</c:v>
+                  <c:v>1880648.5941572969</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3585405.257769749</c:v>
+                  <c:v>3886673.761258414</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1314,19 +1436,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>106276.44246872517</c:v>
+                  <c:v>-18399.200105876836</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>184857.53890245035</c:v>
+                  <c:v>88578.172732066188</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>342019.73176990077</c:v>
+                  <c:v>302532.91840795206</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>656344.11750480137</c:v>
+                  <c:v>730442.40975972381</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1284992.8889746028</c:v>
+                  <c:v>1586261.3924632678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3027,11 +3149,11 @@
   </sheetPr>
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3186,9 +3308,12 @@
       </c>
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E26" t="s">
+      <c r="E26" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
     </row>
     <row r="44" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I44" s="3"/>
@@ -3260,6 +3385,252 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D477174F-5EB3-D14B-80D0-DCACDF5B81EF}">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B5" sqref="B5:F5"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5:F5"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:F5"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="55.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731DAEB7-84E3-F64E-A6D2-57429C6FFEA3}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -3289,7 +3660,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21880609-280D-7840-884C-B6D9F6A39CDD}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3363,7 +3734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCAD7EB-2781-E14C-90C6-B0A74EB91CBA}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3406,7 +3777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4DB2EF4-5C6D-0F4E-9382-000FC8FE0D80}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3480,7 +3851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C2EF97-D034-D047-982A-FFFC278580D2}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3491,7 +3862,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3618,343 +3989,6 @@
       </c>
       <c r="D9" t="s">
         <v>98</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505FF6CF-6A1B-6E42-BA01-A0AFAB15D317}">
-  <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:D27"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="72.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="11">
-        <v>31.828099999999999</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="4">
-        <f>2.3/7.9</f>
-        <v>0.29113924050632906</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1.40923</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1460000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="5">
-        <f>B5/B4</f>
-        <v>1036026.7663901564</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="5">
-        <v>4440000</v>
-      </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="5">
-        <f>B7*B3*B4</f>
-        <v>1821652.7544303793</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="7">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="D9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="7">
-        <v>0.16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="7">
-        <f>B9*B10</f>
-        <v>9.2799999999999994E-2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="7">
-        <f>177/430</f>
-        <v>0.41162790697674417</v>
-      </c>
-      <c r="D12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0.98</v>
-      </c>
-      <c r="D15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="D16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>136</v>
-      </c>
-      <c r="B17" s="12">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>138</v>
-      </c>
-      <c r="D17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B18" s="12">
-        <f>30</f>
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" s="6">
-        <v>0.72</v>
-      </c>
-      <c r="D19" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>111</v>
-      </c>
-      <c r="B20" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>112</v>
-      </c>
-      <c r="B21" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B22" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="12">
-        <v>3</v>
-      </c>
-      <c r="D23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" s="12">
-        <v>24</v>
-      </c>
-      <c r="D24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="6">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>127</v>
-      </c>
-      <c r="B26" s="6">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="6">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -3992,7 +4026,7 @@
       </c>
       <c r="B2" s="19">
         <f>'Yearly Values &amp; Costs'!B2-'Yearly Values &amp; Costs'!C2</f>
-        <v>106276.44246872517</v>
+        <v>-18399.200105876836</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4001,7 +4035,7 @@
       </c>
       <c r="B3" s="19">
         <f>'Yearly Values &amp; Costs'!B3-'Yearly Values &amp; Costs'!C3</f>
-        <v>184857.53890245035</v>
+        <v>88578.172732066188</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -4010,7 +4044,7 @@
       </c>
       <c r="B4" s="19">
         <f>'Yearly Values &amp; Costs'!B4-'Yearly Values &amp; Costs'!C4</f>
-        <v>342019.73176990077</v>
+        <v>302532.91840795206</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -4019,7 +4053,7 @@
       </c>
       <c r="B5" s="19">
         <f>'Yearly Values &amp; Costs'!B5-'Yearly Values &amp; Costs'!C5</f>
-        <v>656344.11750480137</v>
+        <v>730442.40975972381</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -4028,7 +4062,7 @@
       </c>
       <c r="B6" s="19">
         <f>'Yearly Values &amp; Costs'!B6-'Yearly Values &amp; Costs'!C6</f>
-        <v>1284992.8889746028</v>
+        <v>1586261.3924632678</v>
       </c>
     </row>
   </sheetData>
@@ -4077,8 +4111,8 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <f>'Portfolio Value Summary'!$C$22</f>
-        <v>250052.21551842181</v>
+        <f>'Portfolio Value Summary'!$C$23</f>
+        <v>125376.5729438198</v>
       </c>
       <c r="C2" s="1">
         <f>'Portfolio Cost Summary'!$C$13</f>
@@ -4086,7 +4120,7 @@
       </c>
       <c r="D2" s="17">
         <f>B2-C2</f>
-        <v>106276.44246872517</v>
+        <v>-18399.200105876836</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4094,16 +4128,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <f>'Portfolio Value Summary'!$D$22</f>
-        <v>472409.08500184363</v>
+        <f>'Portfolio Value Summary'!$D$23</f>
+        <v>376129.71883145947</v>
       </c>
       <c r="C3" s="1">
         <f>'Portfolio Cost Summary'!$D$13</f>
         <v>287551.54609939328</v>
       </c>
       <c r="D3" s="17">
-        <f t="shared" ref="D3:D6" si="0">B3-C3</f>
-        <v>184857.53890245035</v>
+        <f>B3-C3</f>
+        <v>88578.172732066188</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4111,16 +4145,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <f>'Portfolio Value Summary'!$E$22</f>
-        <v>917122.82396868733</v>
+        <f>'Portfolio Value Summary'!$E$23</f>
+        <v>877636.01060673862</v>
       </c>
       <c r="C4" s="1">
         <f>'Portfolio Cost Summary'!$E$13</f>
         <v>575103.09219878656</v>
       </c>
       <c r="D4" s="17">
-        <f t="shared" si="0"/>
-        <v>342019.73176990077</v>
+        <f>B4-C4</f>
+        <v>302532.91840795206</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4128,16 +4162,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <f>'Portfolio Value Summary'!$F$22</f>
-        <v>1806550.3019023745</v>
+        <f>'Portfolio Value Summary'!$F$23</f>
+        <v>1880648.5941572969</v>
       </c>
       <c r="C5" s="1">
         <f>'Portfolio Cost Summary'!$F$13</f>
         <v>1150206.1843975731</v>
       </c>
       <c r="D5" s="17">
-        <f t="shared" si="0"/>
-        <v>656344.11750480137</v>
+        <f>B5-C5</f>
+        <v>730442.40975972381</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4145,16 +4179,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <f>'Portfolio Value Summary'!$G$22</f>
-        <v>3585405.257769749</v>
+        <f>'Portfolio Value Summary'!$G$23</f>
+        <v>3886673.761258414</v>
       </c>
       <c r="C6" s="1">
         <f>'Portfolio Cost Summary'!$G$13</f>
         <v>2300412.3687951462</v>
       </c>
       <c r="D6" s="17">
-        <f t="shared" si="0"/>
-        <v>1284992.8889746028</v>
+        <f>B6-C6</f>
+        <v>1586261.3924632678</v>
       </c>
     </row>
     <row r="27" spans="5:5" x14ac:dyDescent="0.2">
@@ -4170,14 +4204,14 @@
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M28" sqref="M28"/>
       <selection pane="topRight" activeCell="M28" sqref="M28"/>
       <selection pane="bottomLeft" activeCell="M28" sqref="M28"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4244,7 +4278,7 @@
         <v>802278.9281216244</v>
       </c>
       <c r="H2" s="11">
-        <f>SUM(C2:G2)</f>
+        <f t="shared" ref="H2:H22" si="0">SUM(C2:G2)</f>
         <v>1554415.4232356474</v>
       </c>
     </row>
@@ -4276,7 +4310,7 @@
         <v>56795.367365599988</v>
       </c>
       <c r="H3" s="11">
-        <f t="shared" ref="H3" si="0">SUM(C3:G3)</f>
+        <f t="shared" si="0"/>
         <v>110041.02427084997</v>
       </c>
     </row>
@@ -4308,7 +4342,7 @@
         <v>4431255.3656000001</v>
       </c>
       <c r="H4" s="11">
-        <f>SUM(C4:G4)</f>
+        <f t="shared" si="0"/>
         <v>8585557.270849999</v>
       </c>
     </row>
@@ -4340,7 +4374,7 @@
         <v>2215627.6828000001</v>
       </c>
       <c r="H5" s="11">
-        <f t="shared" ref="H5:H7" si="1">SUM(C5:G5)</f>
+        <f t="shared" si="0"/>
         <v>4292778.6354249995</v>
       </c>
     </row>
@@ -4372,7 +4406,7 @@
         <v>1329376.60968</v>
       </c>
       <c r="H6" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2575667.1812549997</v>
       </c>
     </row>
@@ -4404,40 +4438,40 @@
         <v>886251.07312000007</v>
       </c>
       <c r="H7" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1717111.4541700003</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C8" s="11">
-        <f>C2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>22564.094853420684</v>
+        <f>(('Value Constants'!$B$17*'Team Hourly Burn'!$B$2)+('Value Constants'!$B$18*'Cost Constants'!$B$4)+('Sensitivity Analysis Variables'!$C$8*'Sensitivity Analysis Variables'!$C$10))*'Value Constants'!$B$28*'Sensitivity Analysis Variables'!C$3*(SUM('Value Constants'!$B$30,'Value Constants'!$B$31))</f>
+        <v>950.41405995633659</v>
       </c>
       <c r="D8" s="11">
-        <f>D2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>45128.189706841367</v>
+        <f>(('Value Constants'!$B$17*'Team Hourly Burn'!$B$2)+('Value Constants'!$B$18*'Cost Constants'!$B$4)+('Sensitivity Analysis Variables'!$C$8*'Sensitivity Analysis Variables'!$C$10))*'Value Constants'!$B$28*'Sensitivity Analysis Variables'!D$3*(SUM('Value Constants'!$B$30,'Value Constants'!$B$31))</f>
+        <v>1900.8281199126732</v>
       </c>
       <c r="E8" s="11">
-        <f>E2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>90256.379413682735</v>
+        <f>(('Value Constants'!$B$17*'Team Hourly Burn'!$B$2)+('Value Constants'!$B$18*'Cost Constants'!$B$4)+('Sensitivity Analysis Variables'!$C$8*'Sensitivity Analysis Variables'!$C$10))*'Value Constants'!$B$28*'Sensitivity Analysis Variables'!E$3*(SUM('Value Constants'!$B$30,'Value Constants'!$B$31))</f>
+        <v>3801.6562398253463</v>
       </c>
       <c r="F8" s="11">
-        <f>F2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>180512.75882736547</v>
+        <f>(('Value Constants'!$B$17*'Team Hourly Burn'!$B$2)+('Value Constants'!$B$18*'Cost Constants'!$B$4)+('Sensitivity Analysis Variables'!$C$8*'Sensitivity Analysis Variables'!$C$10))*'Value Constants'!$B$28*'Sensitivity Analysis Variables'!F$3*(SUM('Value Constants'!$B$30,'Value Constants'!$B$31))</f>
+        <v>7603.3124796506927</v>
       </c>
       <c r="G8" s="11">
-        <f>G2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>361025.51765473094</v>
+        <f>(('Value Constants'!$B$17*'Team Hourly Burn'!$B$2)+('Value Constants'!$B$18*'Cost Constants'!$B$4)+('Sensitivity Analysis Variables'!$C$8*'Sensitivity Analysis Variables'!$C$10))*'Value Constants'!$B$28*'Sensitivity Analysis Variables'!G$3*(SUM('Value Constants'!$B$30,'Value Constants'!$B$31))</f>
+        <v>15206.624959301385</v>
       </c>
       <c r="H8" s="11">
-        <f>SUM(C8:G8)</f>
-        <v>699486.94045604113</v>
+        <f t="shared" si="0"/>
+        <v>29462.835858646435</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -4445,31 +4479,31 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="C9" s="11">
-        <f>C$5*'Value Constants'!$B$20</f>
-        <v>110781.38414000001</v>
+        <f>(C$2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47</f>
+        <v>11282.047426710342</v>
       </c>
       <c r="D9" s="11">
-        <f>D$5*'Value Constants'!$B$20</f>
-        <v>221562.76828000002</v>
+        <f>C$9+((D$2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>33846.142280131025</v>
       </c>
       <c r="E9" s="11">
-        <f>E$5*'Value Constants'!$B$20</f>
-        <v>443125.53656000004</v>
+        <f>D$9+((E$2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>78974.331986972393</v>
       </c>
       <c r="F9" s="11">
-        <f>F$5*'Value Constants'!$B$20</f>
-        <v>886251.07312000007</v>
+        <f>E$9+((F$2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>169230.71140065513</v>
       </c>
       <c r="G9" s="11">
-        <f>G$5*'Value Constants'!$B$20</f>
-        <v>1772502.1462400001</v>
+        <f>F$9+((G$2*('Value Constants'!$B$14-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>349743.47022802057</v>
       </c>
       <c r="H9" s="11">
-        <f t="shared" ref="H9:H20" si="2">SUM(C9:G9)</f>
-        <v>3434222.9083400005</v>
+        <f t="shared" si="0"/>
+        <v>643076.70332248951</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -4477,31 +4511,31 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" s="11">
-        <f>C$6*'Value Constants'!$B$21</f>
-        <v>49851.622862999997</v>
+        <f>(C$5*'Value Constants'!$B$20)/'Value Constants'!$B$47</f>
+        <v>55390.692070000005</v>
       </c>
       <c r="D10" s="11">
-        <f>D$6*'Value Constants'!$B$21</f>
-        <v>99703.245725999994</v>
+        <f>C$10+((D$5*'Value Constants'!$B$20)/'Value Constants'!$B$47)</f>
+        <v>166172.07621000003</v>
       </c>
       <c r="E10" s="11">
-        <f>E$6*'Value Constants'!$B$21</f>
-        <v>199406.49145199999</v>
+        <f>D$10+((E$5*'Value Constants'!$B$20)/'Value Constants'!$B$47)</f>
+        <v>387734.84449000005</v>
       </c>
       <c r="F10" s="11">
-        <f>F$6*'Value Constants'!$B$21</f>
-        <v>398812.98290399997</v>
+        <f>E$10+((F$5*'Value Constants'!$B$20)/'Value Constants'!$B$47)</f>
+        <v>830860.38105000008</v>
       </c>
       <c r="G10" s="11">
-        <f>G$6*'Value Constants'!$B$21</f>
-        <v>797625.96580799995</v>
+        <f>F$10+((G$5*'Value Constants'!$B$20)/'Value Constants'!$B$47)</f>
+        <v>1717111.4541700003</v>
       </c>
       <c r="H10" s="11">
-        <f>SUM(C10:G10)</f>
-        <v>1545400.3087529999</v>
+        <f t="shared" si="0"/>
+        <v>3157269.4479900002</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -4509,31 +4543,31 @@
         <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C11" s="11">
-        <f>$C$7*'Value Constants'!$B$22</f>
-        <v>27695.346035000002</v>
+        <f>(C$6*'Value Constants'!$B$21)/'Value Constants'!$B$47</f>
+        <v>24925.811431499998</v>
       </c>
       <c r="D11" s="11">
-        <f>$C$7*'Value Constants'!$B$22</f>
-        <v>27695.346035000002</v>
+        <f>C$11+((D$6*'Value Constants'!$B$21)/'Value Constants'!$B$47)</f>
+        <v>74777.434294499995</v>
       </c>
       <c r="E11" s="11">
-        <f>$C$7*'Value Constants'!$B$22</f>
-        <v>27695.346035000002</v>
+        <f>D$11+((E$6*'Value Constants'!$B$21)/'Value Constants'!$B$47)</f>
+        <v>174480.68002049997</v>
       </c>
       <c r="F11" s="11">
-        <f>$C$7*'Value Constants'!$B$22</f>
-        <v>27695.346035000002</v>
+        <f>E$11+((F$6*'Value Constants'!$B$21)/'Value Constants'!$B$47)</f>
+        <v>373887.17147249996</v>
       </c>
       <c r="G11" s="11">
-        <f>$C$7*'Value Constants'!$B$22</f>
-        <v>27695.346035000002</v>
+        <f>F$11+((G$6*'Value Constants'!$B$21)/'Value Constants'!$B$47)</f>
+        <v>772700.15437649994</v>
       </c>
       <c r="H11" s="11">
-        <f t="shared" si="2"/>
-        <v>138476.730175</v>
+        <f t="shared" si="0"/>
+        <v>1420771.2515954999</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -4541,87 +4575,99 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+        <v>101</v>
+      </c>
+      <c r="C12" s="11">
+        <f>(C$7*'Value Constants'!$B$22)/'Value Constants'!$B$47</f>
+        <v>13847.673017500001</v>
+      </c>
+      <c r="D12" s="11">
+        <f>C$12+((D$7*'Value Constants'!$B$22)/'Value Constants'!$B$47)</f>
+        <v>41543.019052500007</v>
+      </c>
+      <c r="E12" s="11">
+        <f>D$12+((E$7*'Value Constants'!$B$22)/'Value Constants'!$B$47)</f>
+        <v>96933.711122500012</v>
+      </c>
+      <c r="F12" s="11">
+        <f>E$12+((F$7*'Value Constants'!$B$22)/'Value Constants'!$B$47)</f>
+        <v>207715.09526250002</v>
+      </c>
+      <c r="G12" s="11">
+        <f>F$12+((G$7*'Value Constants'!$B$22)/'Value Constants'!$B$47)</f>
+        <v>429277.86354250007</v>
+      </c>
+      <c r="H12" s="11">
+        <f t="shared" si="0"/>
+        <v>789317.36199750006</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="H13" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="H14" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+      <c r="H15" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="11">
-        <f>C2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>36603.976095549115</v>
-      </c>
-      <c r="D16" s="11">
-        <f>D2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>73207.952191098229</v>
-      </c>
-      <c r="E16" s="11">
-        <f>E2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>146415.90438219646</v>
-      </c>
-      <c r="F16" s="11">
-        <f>F2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>292831.80876439292</v>
-      </c>
-      <c r="G16" s="11">
-        <f>G2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16)</f>
-        <v>585663.61752878584</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="11">
-        <f t="shared" si="2"/>
-        <v>1134723.2589620226</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -4629,31 +4675,31 @@
         <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="C17" s="11">
-        <f>'Portfolio Value Summary'!C$3*'Value Constants'!$B$19</f>
-        <v>2555.7915314519992</v>
+        <f>(C$2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47</f>
+        <v>18301.988047774557</v>
       </c>
       <c r="D17" s="11">
-        <f>'Portfolio Value Summary'!D$3*'Value Constants'!$B$19</f>
-        <v>5111.5830629039983</v>
+        <f>C$17+((D$2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>54905.964143323668</v>
       </c>
       <c r="E17" s="11">
-        <f>'Portfolio Value Summary'!E$3*'Value Constants'!$B$19</f>
-        <v>10223.166125807997</v>
+        <f>D$17+((E$2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>128113.9163344219</v>
       </c>
       <c r="F17" s="11">
-        <f>'Portfolio Value Summary'!F$3*'Value Constants'!$B$19</f>
-        <v>20446.332251615993</v>
+        <f>E$17+((F$2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>274529.82071661833</v>
       </c>
       <c r="G17" s="11">
-        <f>'Portfolio Value Summary'!G$3*'Value Constants'!$B$19</f>
-        <v>40892.664503231987</v>
+        <f>F$17+((G$2*('Value Constants'!$B$15-'Value Constants'!$B$13-'Value Constants'!$B$16))/'Value Constants'!$B$47)</f>
+        <v>567361.6294810113</v>
       </c>
       <c r="H17" s="11">
-        <f>SUM(C17:G17)</f>
-        <v>79229.537475011981</v>
+        <f t="shared" si="0"/>
+        <v>1043213.3187231498</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -4661,16 +4707,31 @@
         <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+        <v>129</v>
+      </c>
+      <c r="C18" s="11">
+        <f>('Portfolio Value Summary'!C$3*'Value Constants'!$B$19)/'Value Constants'!$B$47</f>
+        <v>1277.8957657259996</v>
+      </c>
+      <c r="D18" s="11">
+        <f>C$18+(('Portfolio Value Summary'!D$3*'Value Constants'!$B$19)/'Value Constants'!$B$47)</f>
+        <v>3833.6872971779985</v>
+      </c>
+      <c r="E18" s="11">
+        <f>D$18+(('Portfolio Value Summary'!E$3*'Value Constants'!$B$19)/'Value Constants'!$B$47)</f>
+        <v>8945.2703600819968</v>
+      </c>
+      <c r="F18" s="11">
+        <f>E$18+(('Portfolio Value Summary'!F$3*'Value Constants'!$B$19)/'Value Constants'!$B$47)</f>
+        <v>19168.436485889993</v>
+      </c>
+      <c r="G18" s="11">
+        <f>F$18+(('Portfolio Value Summary'!G$3*'Value Constants'!$B$19)/'Value Constants'!$B$47)</f>
+        <v>39614.76873750599</v>
+      </c>
       <c r="H18" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>72840.058646381978</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -4678,16 +4739,31 @@
         <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+        <v>102</v>
+      </c>
+      <c r="C19" s="11">
+        <f>((1-('Value Constants'!$B$29/'Value Constants'!$B$28))*'Portfolio Value Summary'!C$8)/'Value Constants'!$B$47</f>
+        <v>350.46518460889916</v>
+      </c>
+      <c r="D19" s="11">
+        <f>C$19+(((1-('Value Constants'!$B$29/'Value Constants'!$B$28))*'Portfolio Value Summary'!D$8)/'Value Constants'!$B$47)</f>
+        <v>1051.3955538266976</v>
+      </c>
+      <c r="E19" s="11">
+        <f>D$19+(((1-('Value Constants'!$B$29/'Value Constants'!$B$28))*'Portfolio Value Summary'!E$8)/'Value Constants'!$B$47)</f>
+        <v>2453.2562922622942</v>
+      </c>
+      <c r="F19" s="11">
+        <f>E$19+(((1-('Value Constants'!$B$29/'Value Constants'!$B$28))*'Portfolio Value Summary'!F$8)/'Value Constants'!$B$47)</f>
+        <v>5256.9777691334875</v>
+      </c>
+      <c r="G19" s="11">
+        <f>F$19+(((1-('Value Constants'!$B$29/'Value Constants'!$B$28))*'Portfolio Value Summary'!G$8)/'Value Constants'!$B$47)</f>
+        <v>10864.420722875875</v>
+      </c>
       <c r="H19" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>19976.515522707254</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -4695,7 +4771,7 @@
         <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -4703,7 +4779,7 @@
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -4712,42 +4788,62 @@
         <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
+      <c r="H21" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="11">
-        <f>SUM(C8:C20)</f>
-        <v>250052.21551842181</v>
-      </c>
-      <c r="D22" s="11">
-        <f>SUM(D8:D20)</f>
-        <v>472409.08500184363</v>
-      </c>
-      <c r="E22" s="11">
-        <f>SUM(E8:E20)</f>
-        <v>917122.82396868733</v>
-      </c>
-      <c r="F22" s="11">
-        <f>SUM(F8:F20)</f>
-        <v>1806550.3019023745</v>
-      </c>
-      <c r="G22" s="11">
-        <f>SUM(G8:G20)</f>
-        <v>3585405.257769749</v>
-      </c>
-      <c r="H22" s="11">
-        <f>SUM(C22:G22)</f>
-        <v>7031539.6841610763</v>
+      <c r="C23" s="11">
+        <f>SUM(C9:C21)</f>
+        <v>125376.5729438198</v>
+      </c>
+      <c r="D23" s="11">
+        <f>SUM(D9:D21)</f>
+        <v>376129.71883145947</v>
+      </c>
+      <c r="E23" s="11">
+        <f>SUM(E9:E21)</f>
+        <v>877636.01060673862</v>
+      </c>
+      <c r="F23" s="11">
+        <f>SUM(F9:F21)</f>
+        <v>1880648.5941572969</v>
+      </c>
+      <c r="G23" s="11">
+        <f>SUM(G9:G21)</f>
+        <v>3886673.761258414</v>
+      </c>
+      <c r="H23" s="11">
+        <f>SUM(C23:G23)</f>
+        <v>7146464.6577977287</v>
       </c>
     </row>
   </sheetData>
@@ -4756,6 +4852,607 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505FF6CF-6A1B-6E42-BA01-A0AFAB15D317}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:D47"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B47" sqref="B47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="72.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="11">
+        <v>31.828099999999999</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="4">
+        <f>2.3/7.9</f>
+        <v>0.29113924050632906</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1.40923</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1460000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="5">
+        <f>B5/B4</f>
+        <v>1036026.7663901564</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="5">
+        <v>4440000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="5">
+        <f>B7*B3*B4</f>
+        <v>1821652.7544303793</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="7">
+        <f>B9*B10</f>
+        <v>9.2799999999999994E-2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="7">
+        <f>177/430</f>
+        <v>0.41162790697674417</v>
+      </c>
+      <c r="D12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0.98</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="D16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="12">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" s="12">
+        <f>30</f>
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="D19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="12">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="12">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>145</v>
+      </c>
+      <c r="B28" s="12">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>147</v>
+      </c>
+      <c r="D28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="12">
+        <v>2.1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30">
+        <f>1/2475</f>
+        <v>4.0404040404040404E-4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>151</v>
+      </c>
+      <c r="D30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="12">
+        <f>1/10</f>
+        <v>0.1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B32" s="12">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="20">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="D33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="12">
+        <v>51</v>
+      </c>
+      <c r="C34" t="s">
+        <v>158</v>
+      </c>
+      <c r="D34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35" s="12">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>160</v>
+      </c>
+      <c r="B36" s="12">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="12">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>165</v>
+      </c>
+      <c r="B38" s="12">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="12">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>170</v>
+      </c>
+      <c r="B40" s="12">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>171</v>
+      </c>
+      <c r="B41" s="12">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>173</v>
+      </c>
+      <c r="B42" s="12">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B43" s="12">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" s="12">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>181</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D4432B-F9B7-BD4A-9D67-F31606253D99}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -5177,19 +5874,19 @@
         <v>143775.77304969664</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="D13:G13" si="1">SUM(D2:D12)</f>
+        <f>SUM(D2:D12)</f>
         <v>287551.54609939328</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="1"/>
+        <f>SUM(E2:E12)</f>
         <v>575103.09219878656</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
+        <f>SUM(F2:F12)</f>
         <v>1150206.1843975731</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="1"/>
+        <f>SUM(G2:G12)</f>
         <v>2300412.3687951462</v>
       </c>
       <c r="H13" s="1">
@@ -5202,7 +5899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1226F3-B512-544C-9A73-84F0129838E2}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -5244,7 +5941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6621B249-8CC2-E94D-9485-1BC74B88D830}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -5268,13 +5965,13 @@
       <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -5338,14 +6035,14 @@
         <f>Dashboard!$C3</f>
         <v>10% Employees</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="21">
         <f>IF('Sensitity Analysis Dropdowns'!$B$5='Sensitivity Analysis Variables'!$B4, 'Sensitity Analysis Constants'!$B$5, IF('Sensitity Analysis Dropdowns'!$B$6='Sensitivity Analysis Variables'!$B4, 'Sensitity Analysis Constants'!$B$6, 'Sensitity Analysis Constants'!$B$7))</f>
         <v>0.1</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
@@ -5356,14 +6053,14 @@
         <f>Dashboard!$C4</f>
         <v>Trained by Working on Previous Teams</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="21">
         <f>IF('Sensitity Analysis Dropdowns'!$B$8='Sensitivity Analysis Variables'!$B5, 'Sensitity Analysis Constants'!$B$8, IF('Sensitity Analysis Dropdowns'!$B$9='Sensitivity Analysis Variables'!$B5, 'Sensitity Analysis Constants'!$B$9, 'Sensitity Analysis Constants'!$B$10))</f>
         <v>1</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
@@ -5374,14 +6071,14 @@
         <f>Dashboard!$C5</f>
         <v>Medium</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="21">
         <f>IF('Sensitity Analysis Dropdowns'!$B$11='Sensitivity Analysis Variables'!$B6, 'Sensitity Analysis Constants'!$B$11, IF('Sensitity Analysis Dropdowns'!$B$12='Sensitivity Analysis Variables'!$B6, 'Sensitity Analysis Constants'!$B$12, 'Sensitity Analysis Constants'!$B$13))</f>
         <v>0.65</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
@@ -5410,14 +6107,14 @@
         <f>Dashboard!$C7</f>
         <v>5</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="23">
         <f>IF('Sensitity Analysis Dropdowns'!$B$17='Sensitivity Analysis Variables'!$B8, 'Sensitity Analysis Constants'!B$17, IF('Sensitity Analysis Dropdowns'!$B$18='Sensitivity Analysis Variables'!$B8, 'Sensitity Analysis Constants'!$B$18, 'Sensitity Analysis Constants'!$B$19))</f>
         <v>5</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
@@ -5428,14 +6125,14 @@
         <f>Dashboard!$C8</f>
         <v>3 hours</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="23">
         <f>IF('Sensitity Analysis Dropdowns'!$B$20='Sensitivity Analysis Variables'!$B9, 'Sensitity Analysis Constants'!B$20, IF('Sensitity Analysis Dropdowns'!$B$21='Sensitivity Analysis Variables'!$B9, 'Sensitity Analysis Constants'!B21, 'Sensitity Analysis Constants'!B22))</f>
         <v>3</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
@@ -5464,14 +6161,14 @@
         <f>Dashboard!$C10</f>
         <v>Low (3000)</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="21">
         <f>IF('Sensitity Analysis Dropdowns'!$B$26='Sensitivity Analysis Variables'!$B11, 'Sensitity Analysis Constants'!B$26, IF('Sensitity Analysis Dropdowns'!$B$27='Sensitivity Analysis Variables'!$B11, 'Sensitity Analysis Constants'!$B$27, 'Sensitity Analysis Constants'!$B$28))</f>
         <v>3000</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5489,7 +6186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1E70E2-DD7C-2F49-82BE-73E99E27C39B}">
   <dimension ref="A1:H28"/>
   <sheetViews>
@@ -5539,15 +6236,15 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:F2" si="0">C2*2</f>
+        <f>C2*2</f>
         <v>4</v>
       </c>
       <c r="E2">
-        <f t="shared" si="0"/>
+        <f>D2*2</f>
         <v>8</v>
       </c>
       <c r="F2">
-        <f t="shared" si="0"/>
+        <f>E2*2</f>
         <v>16</v>
       </c>
       <c r="H2" t="s">
@@ -5563,19 +6260,19 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:F4" si="1">B3*2</f>
+        <f t="shared" ref="C3:F4" si="0">B3*2</f>
         <v>4</v>
       </c>
       <c r="D3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="H3" t="s">
@@ -5591,19 +6288,19 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
@@ -5615,10 +6312,10 @@
       <c r="B5" s="24">
         <v>0.1</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
@@ -5628,10 +6325,10 @@
       <c r="B6" s="24">
         <v>0.5</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
@@ -5641,49 +6338,49 @@
       <c r="B7" s="24">
         <v>0.9</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A8, " - ", 'Sensitity Analysis Dropdowns'!$B8)</f>
         <v>Experience of Teams with BC Gov Migrations - Figuring it out from Scratch</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="21">
         <v>1.5</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A9, " - ", 'Sensitity Analysis Dropdowns'!$B9)</f>
         <v>Experience of Teams with BC Gov Migrations - Following Best Practice Documents</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="21">
         <v>1.3</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A10, " - ", 'Sensitity Analysis Dropdowns'!$B10)</f>
         <v>Experience of Teams with BC Gov Migrations - Trained by Working on Previous Teams</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="21">
         <v>1</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
@@ -5693,10 +6390,10 @@
       <c r="B11" s="24">
         <v>0.25</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
@@ -5706,10 +6403,10 @@
       <c r="B12" s="24">
         <v>0.65</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
@@ -5719,10 +6416,10 @@
       <c r="B13" s="24">
         <v>0.9</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
@@ -5743,14 +6440,14 @@
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A15, " - ", 'Sensitity Analysis Dropdowns'!$B15)</f>
         <v>Average Cost of Gov Data Breach - Medium</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="25">
         <f>($B$16+$B$14)/2</f>
         <v>1640826.3772151896</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
@@ -5771,78 +6468,78 @@
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A17, " - ", 'Sensitity Analysis Dropdowns'!$B17)</f>
         <v>Average Currently Online Public Users per Application - 5</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="23">
         <v>5</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A18, " - ", 'Sensitity Analysis Dropdowns'!$B18)</f>
         <v>Average Currently Online Public Users per Application - 20</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="23">
         <v>20</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A19, " - ", 'Sensitity Analysis Dropdowns'!$B19)</f>
         <v>Average Currently Online Public Users per Application - 100</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="23">
         <v>100</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A20, " - ", 'Sensitity Analysis Dropdowns'!$B20)</f>
         <v>Average Legacy System Outage Length - 3 hours</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="23">
         <v>3</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A21, " - ", 'Sensitity Analysis Dropdowns'!$B21)</f>
         <v>Average Legacy System Outage Length - 10 hours</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="23">
         <v>10</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A22, " - ", 'Sensitity Analysis Dropdowns'!$B22)</f>
         <v>Average Legacy System Outage Length - 100 hours</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="23">
         <v>100</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
@@ -5888,313 +6585,67 @@
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A26, " - ", 'Sensitity Analysis Dropdowns'!$B26)</f>
         <v>Average Yearly Project Hours on New Features - Low (3000)</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="21">
         <v>3000</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A27, " - ", 'Sensitity Analysis Dropdowns'!$B27)</f>
         <v>Average Yearly Project Hours on New Features - Medium (7500)</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="21">
         <v>7500</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f>_xlfn.CONCAT('Sensitity Analysis Dropdowns'!$A28, " - ", 'Sensitity Analysis Dropdowns'!$B28)</f>
         <v>Average Yearly Project Hours on New Features - High (12000)</v>
       </c>
-      <c r="B28" s="20">
+      <c r="B28" s="21">
         <v>12000</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D477174F-5EB3-D14B-80D0-DCACDF5B81EF}">
-  <dimension ref="A1:B28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B5" sqref="B5:F5"/>
-      <selection pane="topRight" activeCell="B5" sqref="B5:F5"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5:F5"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="55.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>135</v>
-      </c>
-      <c r="B19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>131</v>
-      </c>
-      <c r="B20" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>131</v>
-      </c>
-      <c r="B21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>131</v>
-      </c>
-      <c r="B22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" s="15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>130</v>
-      </c>
-      <c r="B24" s="15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" s="15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>121</v>
-      </c>
-      <c r="B26" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>121</v>
-      </c>
-      <c r="B27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>